<commit_message>
removed thermocouples out of surface
of water, may still need to do more to find the uncertainties?
</commit_message>
<xml_diff>
--- a/uncertainty_pelletwater.xlsx
+++ b/uncertainty_pelletwater.xlsx
@@ -500,16 +500,16 @@
     </row>
     <row r="4">
       <c r="A4" t="n">
-        <v>0.6472226870551324</v>
+        <v>0.6428759570744059</v>
       </c>
       <c r="B4" t="n">
-        <v>0.6445490598851663</v>
+        <v>0.6444263053706816</v>
       </c>
       <c r="C4" t="n">
-        <v>0.6566580352113034</v>
+        <v>0.6451317646088772</v>
       </c>
       <c r="D4" t="n">
-        <v>0.6408907252089526</v>
+        <v>0.6406366763793544</v>
       </c>
       <c r="E4" t="inlineStr">
         <is>
@@ -538,7 +538,7 @@
     </row>
     <row r="6">
       <c r="A6" t="n">
-        <v>0.7683292885642455</v>
+        <v>0.7683220680197399</v>
       </c>
       <c r="B6" t="n">
         <v>0.6444891171670217</v>
@@ -547,7 +547,7 @@
         <v>1.141513708709032</v>
       </c>
       <c r="D6" t="n">
-        <v>0.6403995493807456</v>
+        <v>0.6403939541979988</v>
       </c>
       <c r="E6" t="inlineStr">
         <is>
@@ -557,7 +557,7 @@
     </row>
     <row r="7">
       <c r="A7" t="n">
-        <v>0.7031893796495704</v>
+        <v>0.7031906114146517</v>
       </c>
       <c r="B7" t="n">
         <v>0.6443643000499658</v>
@@ -566,7 +566,7 @@
         <v>0.8601237395359149</v>
       </c>
       <c r="D7" t="n">
-        <v>0.6401396675171226</v>
+        <v>0.6401431656490685</v>
       </c>
       <c r="E7" t="inlineStr">
         <is>

</xml_diff>